<commit_message>
Updated Financial model Practical_19
</commit_message>
<xml_diff>
--- a/Practical_19.xlsx
+++ b/Practical_19.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Financial Model" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -92,10 +92,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +112,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
@@ -198,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,12 +237,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,15 +673,16 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -737,8 +755,26 @@
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <f>((D15-C15)/C15)</f>
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="G5" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="19">
         <v>0.1</v>
       </c>
     </row>
@@ -746,12 +782,30 @@
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <f>C16/C15</f>
         <v>0.45</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <f>D16/D15</f>
+        <v>0.45</v>
+      </c>
+      <c r="E6" s="19">
+        <v>0.45</v>
+      </c>
+      <c r="F6" s="19">
+        <v>0.45</v>
+      </c>
+      <c r="G6" s="19">
+        <v>0.45</v>
+      </c>
+      <c r="H6" s="19">
+        <v>0.45</v>
+      </c>
+      <c r="I6" s="19">
+        <v>0.45</v>
+      </c>
+      <c r="J6" s="19">
         <v>0.45</v>
       </c>
     </row>
@@ -767,18 +821,54 @@
         <f>D18</f>
         <v>18150</v>
       </c>
+      <c r="E7" s="20">
+        <v>19000</v>
+      </c>
+      <c r="F7" s="20">
+        <v>19500</v>
+      </c>
+      <c r="G7" s="20">
+        <v>20000</v>
+      </c>
+      <c r="H7" s="20">
+        <v>20000</v>
+      </c>
+      <c r="I7" s="20">
+        <v>20000</v>
+      </c>
+      <c r="J7" s="20">
+        <v>20000</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="17">
         <f>C20/C15</f>
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="17">
         <f>D20/D15</f>
         <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E8" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="F8" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="G8" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="H8" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="I8" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="J8" s="19">
+        <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -793,17 +883,53 @@
         <f>D21</f>
         <v>1000</v>
       </c>
+      <c r="E9" s="21">
+        <v>1000</v>
+      </c>
+      <c r="F9" s="21">
+        <v>1000</v>
+      </c>
+      <c r="G9" s="21">
+        <v>1000</v>
+      </c>
+      <c r="H9" s="21">
+        <v>1000</v>
+      </c>
+      <c r="I9" s="21">
+        <v>1000</v>
+      </c>
+      <c r="J9" s="21">
+        <v>1000</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="18">
         <f>C23/C22</f>
         <v>0.3</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="18">
         <f>D23/D22</f>
+        <v>0.3</v>
+      </c>
+      <c r="E10" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="F10" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="G10" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="H10" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="I10" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="J10" s="19">
         <v>0.3</v>
       </c>
     </row>
@@ -825,53 +951,143 @@
       <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="22">
         <v>150000</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="22">
         <v>165000</v>
+      </c>
+      <c r="E15" s="23">
+        <f>D15*(E5+1)</f>
+        <v>181500.00000000003</v>
+      </c>
+      <c r="F15" s="23">
+        <f t="shared" ref="F15:J15" si="0">E15*(F5+1)</f>
+        <v>199650.00000000006</v>
+      </c>
+      <c r="G15" s="23">
+        <f t="shared" si="0"/>
+        <v>219615.00000000009</v>
+      </c>
+      <c r="H15" s="23">
+        <f t="shared" si="0"/>
+        <v>241576.50000000012</v>
+      </c>
+      <c r="I15" s="23">
+        <f t="shared" si="0"/>
+        <v>265734.15000000014</v>
+      </c>
+      <c r="J15" s="23">
+        <f t="shared" si="0"/>
+        <v>292307.56500000018</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="22">
         <v>67500</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="22">
         <v>74250</v>
       </c>
+      <c r="E16" s="23">
+        <f>E15*E6</f>
+        <v>81675.000000000015</v>
+      </c>
+      <c r="F16" s="23">
+        <f t="shared" ref="F16:I16" si="1">F15*F6</f>
+        <v>89842.500000000029</v>
+      </c>
+      <c r="G16" s="23">
+        <f t="shared" si="1"/>
+        <v>98826.750000000044</v>
+      </c>
+      <c r="H16" s="23">
+        <f t="shared" si="1"/>
+        <v>108709.42500000006</v>
+      </c>
+      <c r="I16" s="23">
+        <f t="shared" si="1"/>
+        <v>119580.36750000007</v>
+      </c>
+      <c r="J16" s="23">
+        <f>J15*J6</f>
+        <v>131538.40425000008</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17">
+      <c r="B17" s="15"/>
+      <c r="C17" s="24">
         <f>C15-C16</f>
         <v>82500</v>
       </c>
-      <c r="D17" s="17">
-        <f>D15-D16</f>
+      <c r="D17" s="24">
+        <f t="shared" ref="D17:J17" si="2">D15-D16</f>
         <v>90750</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
+      <c r="E17" s="24">
+        <f t="shared" si="2"/>
+        <v>99825.000000000015</v>
+      </c>
+      <c r="F17" s="24">
+        <f t="shared" si="2"/>
+        <v>109807.50000000003</v>
+      </c>
+      <c r="G17" s="24">
+        <f t="shared" si="2"/>
+        <v>120788.25000000004</v>
+      </c>
+      <c r="H17" s="24">
+        <f t="shared" si="2"/>
+        <v>132867.07500000007</v>
+      </c>
+      <c r="I17" s="24">
+        <f t="shared" si="2"/>
+        <v>146153.78250000009</v>
+      </c>
+      <c r="J17" s="24">
+        <f t="shared" si="2"/>
+        <v>160769.1607500001</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="22">
         <v>16500</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="22">
         <v>18150</v>
+      </c>
+      <c r="E18" s="23">
+        <f>E7</f>
+        <v>19000</v>
+      </c>
+      <c r="F18" s="23">
+        <f t="shared" ref="F18:J18" si="3">F7</f>
+        <v>19500</v>
+      </c>
+      <c r="G18" s="23">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="H18" s="23">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="I18" s="23">
+        <f t="shared" si="3"/>
+        <v>20000</v>
+      </c>
+      <c r="J18" s="23">
+        <f t="shared" si="3"/>
+        <v>20000</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -879,30 +1095,72 @@
         <v>5</v>
       </c>
       <c r="B19" s="12"/>
-      <c r="C19" s="12">
+      <c r="C19" s="25">
         <f>C17-C18</f>
         <v>66000</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="25">
         <f>D17-D18</f>
         <v>72600</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
+      <c r="E19" s="25">
+        <f t="shared" ref="E19:J19" si="4">E17-E18</f>
+        <v>80825.000000000015</v>
+      </c>
+      <c r="F19" s="25">
+        <f t="shared" si="4"/>
+        <v>90307.500000000029</v>
+      </c>
+      <c r="G19" s="25">
+        <f t="shared" si="4"/>
+        <v>100788.25000000004</v>
+      </c>
+      <c r="H19" s="25">
+        <f t="shared" si="4"/>
+        <v>112867.07500000007</v>
+      </c>
+      <c r="I19" s="25">
+        <f t="shared" si="4"/>
+        <v>126153.78250000009</v>
+      </c>
+      <c r="J19" s="25">
+        <f t="shared" si="4"/>
+        <v>140769.1607500001</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="22">
         <v>6600</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="22">
         <v>7260</v>
+      </c>
+      <c r="E20" s="23">
+        <f>E8*E15</f>
+        <v>9075.0000000000018</v>
+      </c>
+      <c r="F20" s="23">
+        <f t="shared" ref="F20:J20" si="5">F8*F15</f>
+        <v>9982.5000000000036</v>
+      </c>
+      <c r="G20" s="23">
+        <f t="shared" si="5"/>
+        <v>10980.750000000005</v>
+      </c>
+      <c r="H20" s="23">
+        <f t="shared" si="5"/>
+        <v>12078.825000000006</v>
+      </c>
+      <c r="I20" s="23">
+        <f t="shared" si="5"/>
+        <v>13286.707500000008</v>
+      </c>
+      <c r="J20" s="23">
+        <f t="shared" si="5"/>
+        <v>14615.378250000009</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -910,76 +1168,148 @@
         <v>7</v>
       </c>
       <c r="B21" s="12"/>
-      <c r="C21" s="16">
-        <v>1000</v>
-      </c>
-      <c r="D21" s="16">
-        <v>1000</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
+      <c r="C21" s="26">
+        <v>1000</v>
+      </c>
+      <c r="D21" s="26">
+        <v>1000</v>
+      </c>
+      <c r="E21" s="25">
+        <f>E9</f>
+        <v>1000</v>
+      </c>
+      <c r="F21" s="25">
+        <f t="shared" ref="F21:I21" si="6">F9</f>
+        <v>1000</v>
+      </c>
+      <c r="G21" s="25">
+        <f t="shared" si="6"/>
+        <v>1000</v>
+      </c>
+      <c r="H21" s="25">
+        <f t="shared" si="6"/>
+        <v>1000</v>
+      </c>
+      <c r="I21" s="25">
+        <f t="shared" si="6"/>
+        <v>1000</v>
+      </c>
+      <c r="J21" s="25">
+        <f>J9</f>
+        <v>1000</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="13"/>
-      <c r="C22" s="13">
+      <c r="C22" s="27">
         <f>C19-SUM(C20,C21)</f>
         <v>58400</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="27">
         <f>D19-SUM(D20,D21)</f>
         <v>64340</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
+      <c r="E22" s="27">
+        <f t="shared" ref="E22:J22" si="7">E19-SUM(E20,E21)</f>
+        <v>70750.000000000015</v>
+      </c>
+      <c r="F22" s="27">
+        <f t="shared" si="7"/>
+        <v>79325.000000000029</v>
+      </c>
+      <c r="G22" s="27">
+        <f t="shared" si="7"/>
+        <v>88807.500000000044</v>
+      </c>
+      <c r="H22" s="27">
+        <f t="shared" si="7"/>
+        <v>99788.250000000058</v>
+      </c>
+      <c r="I22" s="27">
+        <f t="shared" si="7"/>
+        <v>111867.07500000008</v>
+      </c>
+      <c r="J22" s="27">
+        <f t="shared" si="7"/>
+        <v>125153.78250000009</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B23" s="12"/>
-      <c r="C23" s="16">
+      <c r="C23" s="26">
         <v>17520</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="26">
         <v>19302</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
+      <c r="E23" s="25">
+        <f>E10*E22</f>
+        <v>21225.000000000004</v>
+      </c>
+      <c r="F23" s="25">
+        <f t="shared" ref="F23:J23" si="8">F10*F22</f>
+        <v>23797.500000000007</v>
+      </c>
+      <c r="G23" s="25">
+        <f t="shared" si="8"/>
+        <v>26642.250000000011</v>
+      </c>
+      <c r="H23" s="25">
+        <f t="shared" si="8"/>
+        <v>29936.475000000017</v>
+      </c>
+      <c r="I23" s="25">
+        <f t="shared" si="8"/>
+        <v>33560.122500000027</v>
+      </c>
+      <c r="J23" s="25">
+        <f t="shared" si="8"/>
+        <v>37546.134750000027</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="14"/>
-      <c r="C24" s="14">
+      <c r="C24" s="28">
         <f>C22-C23</f>
         <v>40880</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="28">
         <f>D22-D23</f>
         <v>45038</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
+      <c r="E24" s="28">
+        <f>E22-E23</f>
+        <v>49525.000000000015</v>
+      </c>
+      <c r="F24" s="28">
+        <f t="shared" ref="E24:J24" si="9">F22-F23</f>
+        <v>55527.500000000022</v>
+      </c>
+      <c r="G24" s="28">
+        <f t="shared" si="9"/>
+        <v>62165.250000000029</v>
+      </c>
+      <c r="H24" s="28">
+        <f>H22-H23</f>
+        <v>69851.775000000038</v>
+      </c>
+      <c r="I24" s="28">
+        <f>I22-I23</f>
+        <v>78306.952500000058</v>
+      </c>
+      <c r="J24" s="28">
+        <f>J22-J23</f>
+        <v>87607.647750000062</v>
+      </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>